<commit_message>
corrigido o erro na hora de fazer a leitura do excel
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/massaDeDados.xlsx
+++ b/src/main/resources/testData/massaDeDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreLuizdaSilva\Documents\curso-BDD-comCucumberEmJava\automacaoPhpTravels\src\main\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27175BDC-942D-4E76-BCC2-07CB1E1AE82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD8054B-44B5-4F2F-9E0F-AFB7E449ECD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{63B6477F-77C6-4442-AE9C-4FB08DA8C217}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{11BE5138-71B5-4D33-9F09-8F62538BD220}"/>
   </bookViews>
   <sheets>
     <sheet name="dadosPessoais" sheetId="1" r:id="rId1"/>
@@ -41,38 +41,38 @@
     <t>id</t>
   </si>
   <si>
+    <t>id_001</t>
+  </si>
+  <si>
     <t>nome</t>
   </si>
   <si>
-    <t>nome da empresa</t>
+    <t>automação</t>
+  </si>
+  <si>
+    <t>sobrenome</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>nomeDaEmpresa</t>
+  </si>
+  <si>
+    <t>world app company</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>id_001</t>
-  </si>
-  <si>
-    <t>automação</t>
-  </si>
-  <si>
-    <t>teste</t>
-  </si>
-  <si>
-    <t>worldwide app company</t>
-  </si>
-  <si>
     <t>emailparatestesautomacao@gmail.com</t>
-  </si>
-  <si>
-    <t>sobrenome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,14 +84,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,10 +110,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -436,60 +427,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2ABB86F-7646-414C-B997-1B05971493D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96BEBF4-1CC6-4E5D-AD97-F01486C12357}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{C9C7CBAC-FF4C-4FB3-BB0B-A01EB23AB583}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{F59A589B-57D5-4A1D-A971-87E022663D48}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>